<commit_message>
working w the data
</commit_message>
<xml_diff>
--- a/combined_responses.xlsx
+++ b/combined_responses.xlsx
@@ -397,251 +397,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>email</v>
-      </c>
-      <c r="C1" t="str">
-        <v>phone</v>
-      </c>
-      <c r="D1" t="str">
-        <v>year</v>
-      </c>
-      <c r="E1" t="str">
-        <v>major</v>
-      </c>
-      <c r="F1" t="str">
-        <v>campus</v>
-      </c>
-      <c r="G1" t="str">
-        <v>timestamp</v>
-      </c>
-      <c r="H1" t="str">
-        <v>form_submitted_at</v>
-      </c>
-      <c r="I1" t="str">
-        <v>quiz_submitted_at</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Genna Gonzaga</v>
-      </c>
-      <c r="B2" t="str">
-        <v>gennasg97@gmail.com</v>
-      </c>
-      <c r="C2" t="str">
-        <v>(929) 684-7039</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2028</v>
-      </c>
-      <c r="E2" t="str">
-        <v>computer science</v>
-      </c>
-      <c r="F2" t="str">
-        <v>Columbia College</v>
-      </c>
-      <c r="G2" t="str">
-        <v>2025-04-01T00:46:16.693Z</v>
-      </c>
-      <c r="H2" t="str">
-        <v>2025-04-01T00:46:16.693Z</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Genna Gonzaga</v>
-      </c>
-      <c r="B3" t="str">
-        <v>gennasg97@gmail.com</v>
-      </c>
-      <c r="C3" t="str">
-        <v>(929) 684-7039</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2027</v>
-      </c>
-      <c r="E3" t="str">
-        <v>computer science</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Columbia College</v>
-      </c>
-      <c r="G3" t="str">
-        <v>2025-04-01T00:46:32.746Z</v>
-      </c>
-      <c r="H3" t="str">
-        <v>2025-04-01T00:46:32.746Z</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Genna Gonzaga</v>
-      </c>
-      <c r="B4" t="str">
-        <v>gennasg97@gmail.com</v>
-      </c>
-      <c r="C4" t="str">
-        <v>(929) 684-7039</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2026</v>
-      </c>
-      <c r="E4" t="str">
-        <v>computer science</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Columbia College</v>
-      </c>
-      <c r="G4" t="str">
-        <v>2025-04-01T00:51:30.537Z</v>
-      </c>
-      <c r="H4" t="str">
-        <v>2025-04-01T00:51:30.537Z</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Genna Gonzaga</v>
-      </c>
-      <c r="B5" t="str">
-        <v>gennasg97@gmail.com</v>
-      </c>
-      <c r="C5" t="str">
-        <v>(929) 684-7039</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2027</v>
-      </c>
-      <c r="E5" t="str">
-        <v>computer science</v>
-      </c>
-      <c r="F5" t="str">
-        <v>Columbia College</v>
-      </c>
-      <c r="G5" t="str">
-        <v>2025-04-01T00:52:00.694Z</v>
-      </c>
-      <c r="H5" t="str">
-        <v>2025-04-01T00:52:00.694Z</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Genna Gonzaga</v>
-      </c>
-      <c r="B6" t="str">
-        <v>gennasg97@gmail.com</v>
-      </c>
-      <c r="C6" t="str">
-        <v>(929) 684-7039</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2027</v>
-      </c>
-      <c r="E6" t="str">
-        <v>computer science</v>
-      </c>
-      <c r="F6" t="str">
-        <v>SEAS</v>
-      </c>
-      <c r="G6" t="str">
-        <v>2025-04-01T00:52:44.777Z</v>
-      </c>
-      <c r="H6" t="str">
-        <v>2025-04-01T00:52:44.777Z</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Genna Gonzaga</v>
-      </c>
-      <c r="B7" t="str">
-        <v>gennasg97@gmail.com</v>
-      </c>
-      <c r="C7" t="str">
-        <v>(929) 684-7039</v>
-      </c>
-      <c r="D7" t="str">
-        <v>2027</v>
-      </c>
-      <c r="E7" t="str">
-        <v>computer science</v>
-      </c>
-      <c r="F7" t="str">
-        <v>Columbia College</v>
-      </c>
-      <c r="G7" t="str">
-        <v>2025-04-01T00:57:40.443Z</v>
-      </c>
-      <c r="H7" t="str">
-        <v>2025-04-01T00:57:40.443Z</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Genna Gonzaga</v>
-      </c>
-      <c r="B8" t="str">
-        <v>gennasg97@gmail.com</v>
-      </c>
-      <c r="C8" t="str">
-        <v>9296847039</v>
-      </c>
-      <c r="D8" t="str">
-        <v>2027</v>
-      </c>
-      <c r="E8" t="str">
-        <v>computer science</v>
-      </c>
-      <c r="F8" t="str">
-        <v>SEAS</v>
-      </c>
-      <c r="G8" t="str">
-        <v>2025-04-21T05:07:14.254Z</v>
-      </c>
-      <c r="H8" t="str">
-        <v>2025-04-21T05:07:14.254Z</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Genna Gonzaga</v>
-      </c>
-      <c r="B9" t="str">
-        <v>gennasg97@gmail.com</v>
-      </c>
-      <c r="C9" t="str">
-        <v>9296847039</v>
-      </c>
-      <c r="D9" t="str">
-        <v>2027</v>
-      </c>
-      <c r="E9" t="str">
-        <v>Computer Science</v>
-      </c>
-      <c r="F9" t="str">
-        <v>SEAS</v>
-      </c>
-      <c r="G9" t="str">
-        <v>2025-04-21T06:00:20.176Z</v>
-      </c>
-      <c r="H9" t="str">
-        <v>2025-04-21T06:00:20.176Z</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>